<commit_message>
Prodution percentage calculation Error fix
</commit_message>
<xml_diff>
--- a/sample/sampleoperator.xlsx
+++ b/sample/sampleoperator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\cnc\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFE4906-704B-4ABF-8EF5-94CA58724FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC6A568-DB3B-4703-9A42-602E3A4BF95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,10 +40,10 @@
     <t>Rework</t>
   </si>
   <si>
-    <t>Diff. %</t>
+    <t>Report Name :- Operator Report</t>
   </si>
   <si>
-    <t>Report Name :- Operator Report</t>
+    <t>Production Percentage</t>
   </si>
 </sst>
 </file>
@@ -613,7 +613,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -623,7 +623,7 @@
     <col min="3" max="3" width="12.85546875" style="1" customWidth="1"/>
     <col min="4" max="5" width="11.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="1" customWidth="1"/>
     <col min="8" max="16" width="12.28515625" style="1"/>
     <col min="17" max="17" width="12.28515625" style="5"/>
     <col min="18" max="18" width="12.28515625" style="2"/>
@@ -654,7 +654,7 @@
       <c r="A4" s="11"/>
       <c r="B4" s="7"/>
       <c r="D4" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
@@ -692,7 +692,7 @@
         <v>5</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>